<commit_message>
Multiple Suite report generation.
</commit_message>
<xml_diff>
--- a/src/test/resources/com/happiestmind/data/SmokeTests.xlsx
+++ b/src/test/resources/com/happiestmind/data/SmokeTests.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="18">
   <si>
     <t>TCID</t>
   </si>
@@ -557,7 +557,7 @@
   <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView showRuler="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -604,7 +604,7 @@
         <v>3</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:6">
@@ -624,7 +624,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>

</xml_diff>